<commit_message>
add converting_docx_to_txt upd replacing_word function change names of txt files in convertin to txt functions
</commit_message>
<xml_diff>
--- a/reports/xlsx/archangelsk.xlsx
+++ b/reports/xlsx/archangelsk.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\For_Python\Unstructured-field-data-aggregator\reports\xlsx\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t>Месторождение</t>
   </si>
@@ -43,6 +48,9 @@
     <t>пористость</t>
   </si>
   <si>
+    <t>КИН</t>
+  </si>
+  <si>
     <t>Архангельское месторождение</t>
   </si>
   <si>
@@ -88,22 +96,28 @@
     <t>81,6</t>
   </si>
   <si>
+    <t>73,4</t>
+  </si>
+  <si>
     <t>76,5</t>
   </si>
   <si>
     <t>70,1</t>
   </si>
   <si>
+    <t>86,5</t>
+  </si>
+  <si>
     <t>68,9</t>
   </si>
   <si>
-    <t>19,3</t>
-  </si>
-  <si>
-    <t>18,7</t>
-  </si>
-  <si>
-    <t>69,3</t>
+    <t>29.5</t>
+  </si>
+  <si>
+    <t>18,6</t>
+  </si>
+  <si>
+    <t>15,2</t>
   </si>
   <si>
     <t>13,5</t>
@@ -116,13 +130,31 @@
   </si>
   <si>
     <t>12,6</t>
+  </si>
+  <si>
+    <t>0,360 доли единиц</t>
+  </si>
+  <si>
+    <t>0,250 доли единиц</t>
+  </si>
+  <si>
+    <t>0,291 долей единиц 0,210 долей единиц 0,250 долей единиц</t>
+  </si>
+  <si>
+    <t>0,270 доли единиц</t>
+  </si>
+  <si>
+    <t>0,465 доли единиц</t>
+  </si>
+  <si>
+    <t>0,316 доли единиц</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,24 +206,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -229,9 +272,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -263,9 +306,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -297,9 +341,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -472,200 +517,249 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="1"/>
+    <col min="9" max="9" width="19.21875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2">
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1">
         <v>4</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1">
+        <v>8</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="1">
+        <v>12</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="1">
+        <v>9</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="1">
+        <v>20</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="1">
+        <v>7</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="1">
+        <v>13</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I2" t="s">
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3">
-        <v>8</v>
-      </c>
-      <c r="H3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5">
-        <v>9</v>
-      </c>
-      <c r="H5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6">
-        <v>20</v>
-      </c>
-      <c r="H6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7">
-        <v>7</v>
-      </c>
-      <c r="H7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="1">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8">
-        <v>13</v>
-      </c>
-      <c r="H8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9" t="s">
-        <v>21</v>
+      <c r="K9" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add kvit tag making
</commit_message>
<xml_diff>
--- a/reports/xlsx/archangelsk.xlsx
+++ b/reports/xlsx/archangelsk.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\For_Python\Unstructured-field-data-aggregator\reports\xlsx\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
   <si>
     <t>Месторождение</t>
   </si>
@@ -49,6 +44,9 @@
   </si>
   <si>
     <t>КИН</t>
+  </si>
+  <si>
+    <t>Квыт</t>
   </si>
   <si>
     <t>Архангельское месторождение</t>
@@ -153,8 +151,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,35 +204,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -272,9 +259,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -306,10 +293,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,10 +327,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -517,249 +502,236 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="28.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="1"/>
-    <col min="9" max="9" width="19.21875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
+    <row r="1" spans="1:12">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="1">
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2">
         <v>4</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5">
+        <v>9</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8">
+        <v>13</v>
+      </c>
+      <c r="H8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" t="s">
+        <v>37</v>
+      </c>
+      <c r="K8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="1">
-        <v>8</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="1">
-        <v>12</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="1">
-        <v>9</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="1">
-        <v>20</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="1">
-        <v>7</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="1">
-        <v>13</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>42</v>
+      <c r="K9" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>